<commit_message>
Updated branch with Simon's fora code.
</commit_message>
<xml_diff>
--- a/diagram tingest.xlsx
+++ b/diagram tingest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Bruger</t>
   </si>
@@ -75,7 +75,22 @@
     <t>*</t>
   </si>
   <si>
-    <t>Admin_ID</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>admin_ID</t>
+  </si>
+  <si>
+    <t>1NF er opfyldt da vi kun har en-værdi-attributter og alle tabeller har en primær nøgle</t>
+  </si>
+  <si>
+    <t>2NF er også opfyldt da vi ikke har nogle sammensatte kandidatnøgler</t>
+  </si>
+  <si>
+    <t>fornavn</t>
+  </si>
+  <si>
+    <t>3NF er også opfyldt da ingen af vores tabellers attributter afhænger af en kandidatnøgle</t>
   </si>
 </sst>
 </file>
@@ -156,36 +171,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -197,50 +214,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1209675</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="36" name="Lige forbindelse 35"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2428875" y="485775"/>
-          <a:ext cx="3667125" cy="561975"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -261,7 +234,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7934325" y="2200275"/>
+          <a:off x="4886325" y="2581275"/>
           <a:ext cx="1209675" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -541,6 +514,94 @@
         <a:xfrm flipH="1" flipV="1">
           <a:off x="7324726" y="476251"/>
           <a:ext cx="1209674" cy="2514599"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Lige forbindelse 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2447925" y="1419225"/>
+          <a:ext cx="3648075" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1209675</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Lige forbindelse 10"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2428875" y="1409700"/>
+          <a:ext cx="1228725" cy="1943100"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -851,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H21"/>
+  <dimension ref="A2:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -864,177 +925,333 @@
     <col min="14" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
+    <row r="2" spans="1:9">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:8">
-      <c r="E3" s="10" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="5"/>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="5"/>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="5"/>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="5"/>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="5"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="5"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="5"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="5"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="D4" s="11"/>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="F5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="B6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="F6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="F7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8">
-      <c r="B8" s="3"/>
-      <c r="D8" s="11"/>
-      <c r="F8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="B9" s="3"/>
-      <c r="D9" s="11"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="2:8">
-      <c r="B10" s="3"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="B11" s="3"/>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="2:8">
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="2:8">
-      <c r="D13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8">
-      <c r="D14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8">
-      <c r="C15" s="10" t="s">
+      <c r="F17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8">
-      <c r="D16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="D17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="D18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="D19" s="3"/>
-      <c r="F19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="9" t="s">
+      <c r="D18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="5"/>
+      <c r="B20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="F20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="9"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="5"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="D22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="D24" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
opret traade navne rettet
</commit_message>
<xml_diff>
--- a/diagram tingest.xlsx
+++ b/diagram tingest.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
-    <sheet name="Ark2" sheetId="2" r:id="rId2"/>
-    <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -1257,28 +1255,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>